<commit_message>
add account number to staff model
</commit_message>
<xml_diff>
--- a/src/tests/integration/__tests__/testFiles/validExcel.xlsx
+++ b/src/tests/integration/__tests__/testFiles/validExcel.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>TN201234</t>
   </si>
@@ -31,6 +31,9 @@
     <t>08034567890</t>
   </si>
   <si>
+    <t>0034567890</t>
+  </si>
+  <si>
     <t>TN201235</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t>08034567891</t>
   </si>
   <si>
+    <t>0034567891</t>
+  </si>
+  <si>
     <t>TN201236</t>
   </si>
   <si>
@@ -61,6 +67,9 @@
     <t>08034567892</t>
   </si>
   <si>
+    <t>0034567892</t>
+  </si>
+  <si>
     <t>TN201237</t>
   </si>
   <si>
@@ -76,6 +85,9 @@
     <t>08034567893</t>
   </si>
   <si>
+    <t>0034567893</t>
+  </si>
+  <si>
     <t>TN201238</t>
   </si>
   <si>
@@ -91,6 +103,9 @@
     <t>08034567894</t>
   </si>
   <si>
+    <t>0034567894</t>
+  </si>
+  <si>
     <t>TN201239</t>
   </si>
   <si>
@@ -106,6 +121,9 @@
     <t>08034567895</t>
   </si>
   <si>
+    <t>0034567895</t>
+  </si>
+  <si>
     <t>TN201240</t>
   </si>
   <si>
@@ -121,6 +139,9 @@
     <t>08034567896</t>
   </si>
   <si>
+    <t>0034567896</t>
+  </si>
+  <si>
     <t>TN201241</t>
   </si>
   <si>
@@ -136,6 +157,9 @@
     <t>08034567897</t>
   </si>
   <si>
+    <t>0034567897</t>
+  </si>
+  <si>
     <t>TN201242</t>
   </si>
   <si>
@@ -151,6 +175,9 @@
     <t>08034567898</t>
   </si>
   <si>
+    <t>0034567898</t>
+  </si>
+  <si>
     <t>TN201243</t>
   </si>
   <si>
@@ -164,6 +191,9 @@
   </si>
   <si>
     <t>08034567899</t>
+  </si>
+  <si>
+    <t>0034567899</t>
   </si>
 </sst>
 </file>
@@ -1334,14 +1364,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="14.5" style="1" customWidth="1"/>
-    <col min="7" max="256" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="7" width="14.5" style="1" customWidth="1"/>
+    <col min="8" max="256" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.7" customHeight="1">
@@ -1363,177 +1393,207 @@
       <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
+      <c r="G1" t="s" s="3">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" ht="14.7" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s" s="3">
         <v>3</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="G2" t="s" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="3" ht="14.7" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s" s="3">
         <v>3</v>
       </c>
       <c r="E3" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="G3" t="s" s="3">
+        <v>18</v>
       </c>
     </row>
     <row r="4" ht="14.7" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s" s="3">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s" s="3">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="s" s="3">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s" s="3">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="G4" t="s" s="3">
+        <v>24</v>
       </c>
     </row>
     <row r="5" ht="14.7" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s" s="3">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s" s="3">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s" s="3">
         <v>3</v>
       </c>
       <c r="E5" t="s" s="3">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s" s="3">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="G5" t="s" s="3">
+        <v>30</v>
       </c>
     </row>
     <row r="6" ht="14.7" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s" s="3">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s" s="3">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="s" s="3">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s" s="3">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="G6" t="s" s="3">
+        <v>36</v>
       </c>
     </row>
     <row r="7" ht="14.7" customHeight="1">
       <c r="A7" t="s" s="2">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s" s="3">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s" s="3">
         <v>3</v>
       </c>
       <c r="E7" t="s" s="3">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F7" t="s" s="3">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="G7" t="s" s="3">
+        <v>42</v>
       </c>
     </row>
     <row r="8" ht="14.7" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s" s="3">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="s" s="3">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s" s="3">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="G8" t="s" s="3">
+        <v>48</v>
       </c>
     </row>
     <row r="9" ht="14.7" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s" s="3">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s" s="3">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s" s="3">
         <v>3</v>
       </c>
       <c r="E9" t="s" s="3">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s" s="3">
-        <v>45</v>
+        <v>53</v>
+      </c>
+      <c r="G9" t="s" s="3">
+        <v>54</v>
       </c>
     </row>
     <row r="10" ht="14.7" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="s" s="3">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s" s="3">
-        <v>50</v>
+        <v>59</v>
+      </c>
+      <c r="G10" t="s" s="3">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add staff id and phone number to line manager
</commit_message>
<xml_diff>
--- a/src/tests/integration/__tests__/testFiles/validExcel.xlsx
+++ b/src/tests/integration/__tests__/testFiles/validExcel.xlsx
@@ -1364,14 +1364,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="14.5" style="1" customWidth="1"/>
-    <col min="8" max="256" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="8" width="14.5" style="1" customWidth="1"/>
+    <col min="9" max="256" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.7" customHeight="1">
@@ -1393,7 +1393,8 @@
       <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="3">
+      <c r="G1" s="3"/>
+      <c r="H1" t="s" s="3">
         <v>6</v>
       </c>
     </row>
@@ -1416,7 +1417,8 @@
       <c r="F2" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" s="3"/>
+      <c r="H2" t="s" s="3">
         <v>12</v>
       </c>
     </row>
@@ -1439,7 +1441,8 @@
       <c r="F3" t="s" s="3">
         <v>17</v>
       </c>
-      <c r="G3" t="s" s="3">
+      <c r="G3" s="3"/>
+      <c r="H3" t="s" s="3">
         <v>18</v>
       </c>
     </row>
@@ -1460,7 +1463,8 @@
       <c r="F4" t="s" s="3">
         <v>23</v>
       </c>
-      <c r="G4" t="s" s="3">
+      <c r="G4" s="3"/>
+      <c r="H4" t="s" s="3">
         <v>24</v>
       </c>
     </row>
@@ -1483,7 +1487,8 @@
       <c r="F5" t="s" s="3">
         <v>29</v>
       </c>
-      <c r="G5" t="s" s="3">
+      <c r="G5" s="3"/>
+      <c r="H5" t="s" s="3">
         <v>30</v>
       </c>
     </row>
@@ -1504,7 +1509,8 @@
       <c r="F6" t="s" s="3">
         <v>35</v>
       </c>
-      <c r="G6" t="s" s="3">
+      <c r="G6" s="3"/>
+      <c r="H6" t="s" s="3">
         <v>36</v>
       </c>
     </row>
@@ -1527,7 +1533,8 @@
       <c r="F7" t="s" s="3">
         <v>41</v>
       </c>
-      <c r="G7" t="s" s="3">
+      <c r="G7" s="3"/>
+      <c r="H7" t="s" s="3">
         <v>42</v>
       </c>
     </row>
@@ -1548,7 +1555,8 @@
       <c r="F8" t="s" s="3">
         <v>47</v>
       </c>
-      <c r="G8" t="s" s="3">
+      <c r="G8" s="3"/>
+      <c r="H8" t="s" s="3">
         <v>48</v>
       </c>
     </row>
@@ -1571,7 +1579,8 @@
       <c r="F9" t="s" s="3">
         <v>53</v>
       </c>
-      <c r="G9" t="s" s="3">
+      <c r="G9" s="3"/>
+      <c r="H9" t="s" s="3">
         <v>54</v>
       </c>
     </row>
@@ -1592,7 +1601,8 @@
       <c r="F10" t="s" s="3">
         <v>59</v>
       </c>
-      <c r="G10" t="s" s="3">
+      <c r="G10" s="3"/>
+      <c r="H10" t="s" s="3">
         <v>60</v>
       </c>
     </row>

</xml_diff>